<commit_message>
allow for eppimapper conversion
</commit_message>
<xml_diff>
--- a/raw-data/grouped list of tags.xlsx
+++ b/raw-data/grouped list of tags.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw.sharepoint.com/sites/VaccineAbsandEfficacy/Shared Documents/28_RSV/Artificial_Antibodies/01_Systematic_Review/04_Summaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{4A6C8A7E-1AE1-4820-BE08-98D073EC109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16B9759-A50B-405C-810D-5E8D08F6FC4D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC52B87C-B7C5-FB4B-A8C3-DE83946D7555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-735" windowWidth="29040" windowHeight="15720" xr2:uid="{CF9A2A78-18C9-4270-BDE6-17FE69BE0101}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{CF9A2A78-18C9-4270-BDE6-17FE69BE0101}"/>
   </bookViews>
   <sheets>
     <sheet name="grouped list of tags" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>Category</t>
   </si>
@@ -278,6 +291,12 @@
   </si>
   <si>
     <t>Developer</t>
+  </si>
+  <si>
+    <t>protein subunit and viral vector</t>
+  </si>
+  <si>
+    <t>unusued</t>
   </si>
 </sst>
 </file>
@@ -1145,18 +1164,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABE9033-0E66-4F81-B469-72629A55C689}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:A72"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1172,7 +1191,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1180,7 +1199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1188,7 +1207,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1196,7 +1215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1204,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1212,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -1220,7 +1239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1228,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -1236,7 +1255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -1244,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1260,7 +1279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1268,7 +1287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1276,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1284,7 +1303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1292,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -1300,7 +1319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1308,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -1316,7 +1335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1324,7 +1343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1332,7 +1351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -1340,7 +1359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1348,7 +1367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1356,7 +1375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1364,7 +1383,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1372,7 +1391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1380,7 +1399,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -1388,7 +1407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -1396,7 +1415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1404,7 +1423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1412,7 +1431,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1420,7 +1439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1428,23 +1447,29 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1452,7 +1477,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1468,7 +1493,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1476,7 +1501,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -1484,7 +1509,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1492,7 +1517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1500,7 +1525,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1516,7 +1541,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1524,7 +1549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1532,7 +1557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1540,7 +1565,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1548,7 +1573,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1556,7 +1581,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -1564,7 +1589,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1572,7 +1597,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>75</v>
       </c>
@@ -1580,7 +1605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -1588,7 +1613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -1596,7 +1621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -1604,7 +1629,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -1612,7 +1637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -1620,7 +1645,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -1628,7 +1653,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -1636,7 +1661,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -1644,7 +1669,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -1652,7 +1677,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -1660,7 +1685,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -1668,7 +1693,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -1676,7 +1701,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1684,7 +1709,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1692,7 +1717,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -1700,7 +1725,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1708,7 +1733,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -1716,7 +1741,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -1724,7 +1749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -1738,6 +1763,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086C82A2D3555884CB771BE97E52D3115" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c9dcc003d42a636022c3b3b61993c4c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="940c4600-7d1a-49e1-aa15-219fdccaff2c" xmlns:ns3="4f2fb40f-cad9-42b1-8429-6e3e59365347" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc8e2c746546ed15d0adb7e8e43aeb5" ns2:_="" ns3:_="">
     <xsd:import namespace="940c4600-7d1a-49e1-aa15-219fdccaff2c"/>
@@ -1998,15 +2032,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2021,6 +2046,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28BD9E81-5DD0-4BAA-AEE7-D97A607CA6E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33A1F0C-8CCC-4441-875B-C28A20D819C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2039,14 +2072,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28BD9E81-5DD0-4BAA-AEE7-D97A607CA6E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A26624F-2457-4B44-AFC3-20F3B40F82D9}">
   <ds:schemaRefs>

</xml_diff>